<commit_message>
Text update - see description
- Added missing ~
- PerformanceChart removed
- Added PerformanceChartFinalBigData
- Added BigData performance chapter
</commit_message>
<xml_diff>
--- a/Text/diagrams/PerformanceChartFinalBigData.xlsx
+++ b/Text/diagrams/PerformanceChartFinalBigData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VUT FIT\10. semestr\DIP\Diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E58C3111-9612-4F2D-9A7C-9EF5E3F748CD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9583C75A-84F5-4F10-9259-C1901517423F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15840" windowHeight="7680" xr2:uid="{0731F486-61CF-4A44-ADA1-383D3BC3EEA7}"/>
   </bookViews>
@@ -441,7 +441,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -463,7 +463,6 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -826,7 +825,7 @@
                   <c:v>500000</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>500000</c:v>
+                  <c:v>351631</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -838,310 +837,310 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="102"/>
                 <c:pt idx="0">
-                  <c:v>25</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>29</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>26</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>25</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>29</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>28</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>25</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>29</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>31</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>28</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>26</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>29</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>31</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>26</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>26</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>26</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>30</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="22">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>29</c:v>
-                </c:pt>
                 <c:pt idx="26">
-                  <c:v>30</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>26</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>32</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>26</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>29</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="32">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="33">
                   <c:v>26</c:v>
                 </c:pt>
-                <c:pt idx="33">
-                  <c:v>27</c:v>
-                </c:pt>
                 <c:pt idx="34">
-                  <c:v>28</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>30</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>31</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>27</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="38">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="53">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="39">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>26</c:v>
-                </c:pt>
                 <c:pt idx="54">
-                  <c:v>27</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>29</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>29</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>30</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>25</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>29</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>27</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>30</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="62">
                   <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="63">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="71">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="64">
+                <c:pt idx="72">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="95">
                   <c:v>27</c:v>
                 </c:pt>
-                <c:pt idx="65">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="68">
+                <c:pt idx="96">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="99">
                   <c:v>27</c:v>
                 </c:pt>
-                <c:pt idx="69">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="86">
+                <c:pt idx="100">
                   <c:v>26</c:v>
                 </c:pt>
-                <c:pt idx="87">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>32</c:v>
-                </c:pt>
                 <c:pt idx="101">
-                  <c:v>29</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2335,7 +2334,7 @@
   <dimension ref="B20:D122"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2359,9 +2358,8 @@
       <c r="C21" s="6">
         <v>500000</v>
       </c>
-      <c r="D21" s="9">
-        <f ca="1">RANDBETWEEN(25,32)</f>
-        <v>25</v>
+      <c r="D21" s="4">
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
@@ -2371,9 +2369,8 @@
       <c r="C22" s="7">
         <v>500000</v>
       </c>
-      <c r="D22" s="9">
-        <f t="shared" ref="D22:D85" ca="1" si="0">RANDBETWEEN(25,32)</f>
-        <v>30</v>
+      <c r="D22" s="4">
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
@@ -2383,9 +2380,8 @@
       <c r="C23" s="7">
         <v>500000</v>
       </c>
-      <c r="D23" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+      <c r="D23" s="4">
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
@@ -2395,9 +2391,8 @@
       <c r="C24" s="7">
         <v>500000</v>
       </c>
-      <c r="D24" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+      <c r="D24" s="4">
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
@@ -2407,9 +2402,8 @@
       <c r="C25" s="7">
         <v>500000</v>
       </c>
-      <c r="D25" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+      <c r="D25" s="4">
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
@@ -2419,9 +2413,8 @@
       <c r="C26" s="7">
         <v>500000</v>
       </c>
-      <c r="D26" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+      <c r="D26" s="4">
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
@@ -2431,9 +2424,8 @@
       <c r="C27" s="7">
         <v>500000</v>
       </c>
-      <c r="D27" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+      <c r="D27" s="4">
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
@@ -2443,9 +2435,8 @@
       <c r="C28" s="7">
         <v>500000</v>
       </c>
-      <c r="D28" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+      <c r="D28" s="4">
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
@@ -2455,9 +2446,8 @@
       <c r="C29" s="7">
         <v>500000</v>
       </c>
-      <c r="D29" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>28</v>
+      <c r="D29" s="4">
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
@@ -2467,9 +2457,8 @@
       <c r="C30" s="7">
         <v>500000</v>
       </c>
-      <c r="D30" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+      <c r="D30" s="4">
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
@@ -2479,8 +2468,7 @@
       <c r="C31" s="7">
         <v>500000</v>
       </c>
-      <c r="D31" s="9">
-        <f t="shared" ca="1" si="0"/>
+      <c r="D31" s="4">
         <v>27</v>
       </c>
     </row>
@@ -2491,9 +2479,8 @@
       <c r="C32" s="7">
         <v>500000</v>
       </c>
-      <c r="D32" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+      <c r="D32" s="4">
+        <v>21</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
@@ -2503,9 +2490,8 @@
       <c r="C33" s="7">
         <v>500000</v>
       </c>
-      <c r="D33" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>31</v>
+      <c r="D33" s="4">
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
@@ -2515,9 +2501,8 @@
       <c r="C34" s="7">
         <v>500000</v>
       </c>
-      <c r="D34" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>28</v>
+      <c r="D34" s="4">
+        <v>21</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
@@ -2527,9 +2512,8 @@
       <c r="C35" s="7">
         <v>500000</v>
       </c>
-      <c r="D35" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+      <c r="D35" s="4">
+        <v>22</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
@@ -2539,9 +2523,8 @@
       <c r="C36" s="7">
         <v>500000</v>
       </c>
-      <c r="D36" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+      <c r="D36" s="4">
+        <v>23</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
@@ -2551,9 +2534,8 @@
       <c r="C37" s="7">
         <v>500000</v>
       </c>
-      <c r="D37" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>31</v>
+      <c r="D37" s="4">
+        <v>24</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
@@ -2563,9 +2545,8 @@
       <c r="C38" s="7">
         <v>500000</v>
       </c>
-      <c r="D38" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+      <c r="D38" s="4">
+        <v>24</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
@@ -2575,9 +2556,8 @@
       <c r="C39" s="7">
         <v>500000</v>
       </c>
-      <c r="D39" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+      <c r="D39" s="4">
+        <v>25</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
@@ -2587,9 +2567,8 @@
       <c r="C40" s="7">
         <v>500000</v>
       </c>
-      <c r="D40" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+      <c r="D40" s="4">
+        <v>21</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
@@ -2599,9 +2578,8 @@
       <c r="C41" s="7">
         <v>500000</v>
       </c>
-      <c r="D41" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+      <c r="D41" s="4">
+        <v>21</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
@@ -2611,9 +2589,8 @@
       <c r="C42" s="7">
         <v>500000</v>
       </c>
-      <c r="D42" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+      <c r="D42" s="4">
+        <v>21</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
@@ -2623,9 +2600,8 @@
       <c r="C43" s="7">
         <v>500000</v>
       </c>
-      <c r="D43" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>32</v>
+      <c r="D43" s="4">
+        <v>20</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.25">
@@ -2635,9 +2611,8 @@
       <c r="C44" s="7">
         <v>500000</v>
       </c>
-      <c r="D44" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+      <c r="D44" s="4">
+        <v>21</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.25">
@@ -2647,9 +2622,8 @@
       <c r="C45" s="7">
         <v>500000</v>
       </c>
-      <c r="D45" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+      <c r="D45" s="4">
+        <v>22</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
@@ -2659,9 +2633,8 @@
       <c r="C46" s="7">
         <v>500000</v>
       </c>
-      <c r="D46" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+      <c r="D46" s="4">
+        <v>25</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.25">
@@ -2671,9 +2644,8 @@
       <c r="C47" s="7">
         <v>500000</v>
       </c>
-      <c r="D47" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+      <c r="D47" s="4">
+        <v>24</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.25">
@@ -2683,9 +2655,8 @@
       <c r="C48" s="7">
         <v>500000</v>
       </c>
-      <c r="D48" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+      <c r="D48" s="4">
+        <v>22</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
@@ -2695,9 +2666,8 @@
       <c r="C49" s="7">
         <v>500000</v>
       </c>
-      <c r="D49" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>32</v>
+      <c r="D49" s="4">
+        <v>22</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.25">
@@ -2707,9 +2677,8 @@
       <c r="C50" s="7">
         <v>500000</v>
       </c>
-      <c r="D50" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+      <c r="D50" s="4">
+        <v>22</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
@@ -2719,8 +2688,7 @@
       <c r="C51" s="7">
         <v>500000</v>
       </c>
-      <c r="D51" s="9">
-        <f t="shared" ca="1" si="0"/>
+      <c r="D51" s="4">
         <v>28</v>
       </c>
     </row>
@@ -2731,9 +2699,8 @@
       <c r="C52" s="7">
         <v>500000</v>
       </c>
-      <c r="D52" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+      <c r="D52" s="4">
+        <v>23</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.25">
@@ -2743,9 +2710,8 @@
       <c r="C53" s="7">
         <v>500000</v>
       </c>
-      <c r="D53" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+      <c r="D53" s="4">
+        <v>23</v>
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.25">
@@ -2755,9 +2721,8 @@
       <c r="C54" s="7">
         <v>500000</v>
       </c>
-      <c r="D54" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+      <c r="D54" s="4">
+        <v>26</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
@@ -2767,9 +2732,8 @@
       <c r="C55" s="7">
         <v>500000</v>
       </c>
-      <c r="D55" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>28</v>
+      <c r="D55" s="4">
+        <v>25</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
@@ -2779,9 +2743,8 @@
       <c r="C56" s="7">
         <v>500000</v>
       </c>
-      <c r="D56" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+      <c r="D56" s="4">
+        <v>26</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.25">
@@ -2791,9 +2754,8 @@
       <c r="C57" s="7">
         <v>500000</v>
       </c>
-      <c r="D57" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>31</v>
+      <c r="D57" s="4">
+        <v>24</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.25">
@@ -2803,9 +2765,8 @@
       <c r="C58" s="7">
         <v>500000</v>
       </c>
-      <c r="D58" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+      <c r="D58" s="4">
+        <v>25</v>
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.25">
@@ -2815,9 +2776,8 @@
       <c r="C59" s="7">
         <v>500000</v>
       </c>
-      <c r="D59" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+      <c r="D59" s="4">
+        <v>21</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.25">
@@ -2827,9 +2787,8 @@
       <c r="C60" s="7">
         <v>500000</v>
       </c>
-      <c r="D60" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+      <c r="D60" s="4">
+        <v>21</v>
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.25">
@@ -2839,9 +2798,8 @@
       <c r="C61" s="7">
         <v>500000</v>
       </c>
-      <c r="D61" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>28</v>
+      <c r="D61" s="4">
+        <v>20</v>
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.25">
@@ -2851,9 +2809,8 @@
       <c r="C62" s="7">
         <v>500000</v>
       </c>
-      <c r="D62" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+      <c r="D62" s="4">
+        <v>19</v>
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.25">
@@ -2863,9 +2820,8 @@
       <c r="C63" s="7">
         <v>500000</v>
       </c>
-      <c r="D63" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+      <c r="D63" s="4">
+        <v>22</v>
       </c>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.25">
@@ -2875,9 +2831,8 @@
       <c r="C64" s="7">
         <v>500000</v>
       </c>
-      <c r="D64" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+      <c r="D64" s="4">
+        <v>20</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
@@ -2887,9 +2842,8 @@
       <c r="C65" s="7">
         <v>500000</v>
       </c>
-      <c r="D65" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+      <c r="D65" s="4">
+        <v>23</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.25">
@@ -2899,9 +2853,8 @@
       <c r="C66" s="7">
         <v>500000</v>
       </c>
-      <c r="D66" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+      <c r="D66" s="4">
+        <v>21</v>
       </c>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
@@ -2911,9 +2864,8 @@
       <c r="C67" s="7">
         <v>500000</v>
       </c>
-      <c r="D67" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>28</v>
+      <c r="D67" s="4">
+        <v>20</v>
       </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.25">
@@ -2923,9 +2875,8 @@
       <c r="C68" s="7">
         <v>500000</v>
       </c>
-      <c r="D68" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+      <c r="D68" s="4">
+        <v>20</v>
       </c>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.25">
@@ -2935,9 +2886,8 @@
       <c r="C69" s="7">
         <v>500000</v>
       </c>
-      <c r="D69" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+      <c r="D69" s="4">
+        <v>21</v>
       </c>
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.25">
@@ -2947,9 +2897,8 @@
       <c r="C70" s="7">
         <v>500000</v>
       </c>
-      <c r="D70" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+      <c r="D70" s="4">
+        <v>20</v>
       </c>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
@@ -2959,9 +2908,8 @@
       <c r="C71" s="7">
         <v>500000</v>
       </c>
-      <c r="D71" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>28</v>
+      <c r="D71" s="4">
+        <v>23</v>
       </c>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.25">
@@ -2971,9 +2919,8 @@
       <c r="C72" s="7">
         <v>500000</v>
       </c>
-      <c r="D72" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+      <c r="D72" s="4">
+        <v>23</v>
       </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.25">
@@ -2983,9 +2930,8 @@
       <c r="C73" s="7">
         <v>500000</v>
       </c>
-      <c r="D73" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+      <c r="D73" s="4">
+        <v>24</v>
       </c>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.25">
@@ -2995,9 +2941,8 @@
       <c r="C74" s="7">
         <v>500000</v>
       </c>
-      <c r="D74" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+      <c r="D74" s="4">
+        <v>25</v>
       </c>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.25">
@@ -3007,9 +2952,8 @@
       <c r="C75" s="7">
         <v>500000</v>
       </c>
-      <c r="D75" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+      <c r="D75" s="4">
+        <v>20</v>
       </c>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.25">
@@ -3019,9 +2963,8 @@
       <c r="C76" s="7">
         <v>500000</v>
       </c>
-      <c r="D76" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+      <c r="D76" s="4">
+        <v>21</v>
       </c>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.25">
@@ -3031,9 +2974,8 @@
       <c r="C77" s="7">
         <v>500000</v>
       </c>
-      <c r="D77" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+      <c r="D77" s="4">
+        <v>20</v>
       </c>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.25">
@@ -3043,9 +2985,8 @@
       <c r="C78" s="7">
         <v>500000</v>
       </c>
-      <c r="D78" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+      <c r="D78" s="4">
+        <v>22</v>
       </c>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.25">
@@ -3055,9 +2996,8 @@
       <c r="C79" s="7">
         <v>500000</v>
       </c>
-      <c r="D79" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+      <c r="D79" s="4">
+        <v>19</v>
       </c>
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.25">
@@ -3067,9 +3007,8 @@
       <c r="C80" s="7">
         <v>500000</v>
       </c>
-      <c r="D80" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+      <c r="D80" s="4">
+        <v>24</v>
       </c>
     </row>
     <row r="81" spans="2:4" x14ac:dyDescent="0.25">
@@ -3079,9 +3018,8 @@
       <c r="C81" s="7">
         <v>500000</v>
       </c>
-      <c r="D81" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+      <c r="D81" s="4">
+        <v>23</v>
       </c>
     </row>
     <row r="82" spans="2:4" x14ac:dyDescent="0.25">
@@ -3091,9 +3029,8 @@
       <c r="C82" s="7">
         <v>500000</v>
       </c>
-      <c r="D82" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+      <c r="D82" s="4">
+        <v>22</v>
       </c>
     </row>
     <row r="83" spans="2:4" x14ac:dyDescent="0.25">
@@ -3103,8 +3040,7 @@
       <c r="C83" s="7">
         <v>500000</v>
       </c>
-      <c r="D83" s="9">
-        <f t="shared" ca="1" si="0"/>
+      <c r="D83" s="4">
         <v>25</v>
       </c>
     </row>
@@ -3115,9 +3051,8 @@
       <c r="C84" s="7">
         <v>500000</v>
       </c>
-      <c r="D84" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+      <c r="D84" s="4">
+        <v>24</v>
       </c>
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.25">
@@ -3127,9 +3062,8 @@
       <c r="C85" s="7">
         <v>500000</v>
       </c>
-      <c r="D85" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+      <c r="D85" s="4">
+        <v>24</v>
       </c>
     </row>
     <row r="86" spans="2:4" x14ac:dyDescent="0.25">
@@ -3139,9 +3073,8 @@
       <c r="C86" s="7">
         <v>500000</v>
       </c>
-      <c r="D86" s="9">
-        <f t="shared" ref="D86:D122" ca="1" si="1">RANDBETWEEN(25,32)</f>
-        <v>29</v>
+      <c r="D86" s="4">
+        <v>24</v>
       </c>
     </row>
     <row r="87" spans="2:4" x14ac:dyDescent="0.25">
@@ -3151,9 +3084,8 @@
       <c r="C87" s="7">
         <v>500000</v>
       </c>
-      <c r="D87" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>28</v>
+      <c r="D87" s="4">
+        <v>22</v>
       </c>
     </row>
     <row r="88" spans="2:4" x14ac:dyDescent="0.25">
@@ -3163,9 +3095,8 @@
       <c r="C88" s="7">
         <v>500000</v>
       </c>
-      <c r="D88" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>31</v>
+      <c r="D88" s="4">
+        <v>26</v>
       </c>
     </row>
     <row r="89" spans="2:4" x14ac:dyDescent="0.25">
@@ -3175,9 +3106,8 @@
       <c r="C89" s="7">
         <v>500000</v>
       </c>
-      <c r="D89" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>27</v>
+      <c r="D89" s="4">
+        <v>25</v>
       </c>
     </row>
     <row r="90" spans="2:4" x14ac:dyDescent="0.25">
@@ -3187,9 +3117,8 @@
       <c r="C90" s="7">
         <v>500000</v>
       </c>
-      <c r="D90" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>32</v>
+      <c r="D90" s="4">
+        <v>25</v>
       </c>
     </row>
     <row r="91" spans="2:4" x14ac:dyDescent="0.25">
@@ -3199,9 +3128,8 @@
       <c r="C91" s="7">
         <v>500000</v>
       </c>
-      <c r="D91" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>27</v>
+      <c r="D91" s="4">
+        <v>25</v>
       </c>
     </row>
     <row r="92" spans="2:4" x14ac:dyDescent="0.25">
@@ -3211,9 +3139,8 @@
       <c r="C92" s="7">
         <v>500000</v>
       </c>
-      <c r="D92" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>29</v>
+      <c r="D92" s="4">
+        <v>30</v>
       </c>
     </row>
     <row r="93" spans="2:4" x14ac:dyDescent="0.25">
@@ -3223,9 +3150,8 @@
       <c r="C93" s="7">
         <v>500000</v>
       </c>
-      <c r="D93" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>31</v>
+      <c r="D93" s="4">
+        <v>23</v>
       </c>
     </row>
     <row r="94" spans="2:4" x14ac:dyDescent="0.25">
@@ -3235,9 +3161,8 @@
       <c r="C94" s="7">
         <v>500000</v>
       </c>
-      <c r="D94" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>31</v>
+      <c r="D94" s="4">
+        <v>21</v>
       </c>
     </row>
     <row r="95" spans="2:4" x14ac:dyDescent="0.25">
@@ -3247,9 +3172,8 @@
       <c r="C95" s="7">
         <v>500000</v>
       </c>
-      <c r="D95" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>30</v>
+      <c r="D95" s="4">
+        <v>23</v>
       </c>
     </row>
     <row r="96" spans="2:4" x14ac:dyDescent="0.25">
@@ -3259,9 +3183,8 @@
       <c r="C96" s="7">
         <v>500000</v>
       </c>
-      <c r="D96" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>29</v>
+      <c r="D96" s="4">
+        <v>23</v>
       </c>
     </row>
     <row r="97" spans="2:4" x14ac:dyDescent="0.25">
@@ -3271,9 +3194,8 @@
       <c r="C97" s="7">
         <v>500000</v>
       </c>
-      <c r="D97" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>28</v>
+      <c r="D97" s="4">
+        <v>23</v>
       </c>
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.25">
@@ -3283,9 +3205,8 @@
       <c r="C98" s="7">
         <v>500000</v>
       </c>
-      <c r="D98" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>30</v>
+      <c r="D98" s="4">
+        <v>22</v>
       </c>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.25">
@@ -3295,9 +3216,8 @@
       <c r="C99" s="7">
         <v>500000</v>
       </c>
-      <c r="D99" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>27</v>
+      <c r="D99" s="4">
+        <v>21</v>
       </c>
     </row>
     <row r="100" spans="2:4" x14ac:dyDescent="0.25">
@@ -3307,9 +3227,8 @@
       <c r="C100" s="7">
         <v>500000</v>
       </c>
-      <c r="D100" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>25</v>
+      <c r="D100" s="4">
+        <v>22</v>
       </c>
     </row>
     <row r="101" spans="2:4" x14ac:dyDescent="0.25">
@@ -3319,9 +3238,8 @@
       <c r="C101" s="7">
         <v>500000</v>
       </c>
-      <c r="D101" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>32</v>
+      <c r="D101" s="4">
+        <v>19</v>
       </c>
     </row>
     <row r="102" spans="2:4" x14ac:dyDescent="0.25">
@@ -3331,9 +3249,8 @@
       <c r="C102" s="7">
         <v>500000</v>
       </c>
-      <c r="D102" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>27</v>
+      <c r="D102" s="4">
+        <v>20</v>
       </c>
     </row>
     <row r="103" spans="2:4" x14ac:dyDescent="0.25">
@@ -3343,9 +3260,8 @@
       <c r="C103" s="7">
         <v>500000</v>
       </c>
-      <c r="D103" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>31</v>
+      <c r="D103" s="4">
+        <v>22</v>
       </c>
     </row>
     <row r="104" spans="2:4" x14ac:dyDescent="0.25">
@@ -3355,9 +3271,8 @@
       <c r="C104" s="7">
         <v>500000</v>
       </c>
-      <c r="D104" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>29</v>
+      <c r="D104" s="4">
+        <v>24</v>
       </c>
     </row>
     <row r="105" spans="2:4" x14ac:dyDescent="0.25">
@@ -3367,9 +3282,8 @@
       <c r="C105" s="7">
         <v>500000</v>
       </c>
-      <c r="D105" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>28</v>
+      <c r="D105" s="4">
+        <v>25</v>
       </c>
     </row>
     <row r="106" spans="2:4" x14ac:dyDescent="0.25">
@@ -3379,9 +3293,8 @@
       <c r="C106" s="7">
         <v>500000</v>
       </c>
-      <c r="D106" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>32</v>
+      <c r="D106" s="4">
+        <v>24</v>
       </c>
     </row>
     <row r="107" spans="2:4" x14ac:dyDescent="0.25">
@@ -3391,9 +3304,8 @@
       <c r="C107" s="7">
         <v>500000</v>
       </c>
-      <c r="D107" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>26</v>
+      <c r="D107" s="4">
+        <v>29</v>
       </c>
     </row>
     <row r="108" spans="2:4" x14ac:dyDescent="0.25">
@@ -3403,9 +3315,8 @@
       <c r="C108" s="7">
         <v>500000</v>
       </c>
-      <c r="D108" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>28</v>
+      <c r="D108" s="4">
+        <v>21</v>
       </c>
     </row>
     <row r="109" spans="2:4" x14ac:dyDescent="0.25">
@@ -3415,9 +3326,8 @@
       <c r="C109" s="7">
         <v>500000</v>
       </c>
-      <c r="D109" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>29</v>
+      <c r="D109" s="4">
+        <v>26</v>
       </c>
     </row>
     <row r="110" spans="2:4" x14ac:dyDescent="0.25">
@@ -3427,9 +3337,8 @@
       <c r="C110" s="7">
         <v>500000</v>
       </c>
-      <c r="D110" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>25</v>
+      <c r="D110" s="4">
+        <v>29</v>
       </c>
     </row>
     <row r="111" spans="2:4" x14ac:dyDescent="0.25">
@@ -3439,9 +3348,8 @@
       <c r="C111" s="7">
         <v>500000</v>
       </c>
-      <c r="D111" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>27</v>
+      <c r="D111" s="4">
+        <v>30</v>
       </c>
     </row>
     <row r="112" spans="2:4" x14ac:dyDescent="0.25">
@@ -3451,9 +3359,8 @@
       <c r="C112" s="7">
         <v>500000</v>
       </c>
-      <c r="D112" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>27</v>
+      <c r="D112" s="4">
+        <v>32</v>
       </c>
     </row>
     <row r="113" spans="2:4" x14ac:dyDescent="0.25">
@@ -3463,9 +3370,8 @@
       <c r="C113" s="7">
         <v>500000</v>
       </c>
-      <c r="D113" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>27</v>
+      <c r="D113" s="4">
+        <v>28</v>
       </c>
     </row>
     <row r="114" spans="2:4" x14ac:dyDescent="0.25">
@@ -3475,9 +3381,8 @@
       <c r="C114" s="7">
         <v>500000</v>
       </c>
-      <c r="D114" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>25</v>
+      <c r="D114" s="4">
+        <v>24</v>
       </c>
     </row>
     <row r="115" spans="2:4" x14ac:dyDescent="0.25">
@@ -3487,9 +3392,8 @@
       <c r="C115" s="7">
         <v>500000</v>
       </c>
-      <c r="D115" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>26</v>
+      <c r="D115" s="4">
+        <v>25</v>
       </c>
     </row>
     <row r="116" spans="2:4" x14ac:dyDescent="0.25">
@@ -3499,9 +3403,8 @@
       <c r="C116" s="7">
         <v>500000</v>
       </c>
-      <c r="D116" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>28</v>
+      <c r="D116" s="4">
+        <v>27</v>
       </c>
     </row>
     <row r="117" spans="2:4" x14ac:dyDescent="0.25">
@@ -3511,9 +3414,8 @@
       <c r="C117" s="7">
         <v>500000</v>
       </c>
-      <c r="D117" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>25</v>
+      <c r="D117" s="4">
+        <v>34</v>
       </c>
     </row>
     <row r="118" spans="2:4" x14ac:dyDescent="0.25">
@@ -3523,9 +3425,8 @@
       <c r="C118" s="7">
         <v>500000</v>
       </c>
-      <c r="D118" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>32</v>
+      <c r="D118" s="4">
+        <v>30</v>
       </c>
     </row>
     <row r="119" spans="2:4" x14ac:dyDescent="0.25">
@@ -3535,9 +3436,8 @@
       <c r="C119" s="7">
         <v>500000</v>
       </c>
-      <c r="D119" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>30</v>
+      <c r="D119" s="4">
+        <v>35</v>
       </c>
     </row>
     <row r="120" spans="2:4" x14ac:dyDescent="0.25">
@@ -3547,9 +3447,8 @@
       <c r="C120" s="7">
         <v>500000</v>
       </c>
-      <c r="D120" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>28</v>
+      <c r="D120" s="4">
+        <v>27</v>
       </c>
     </row>
     <row r="121" spans="2:4" x14ac:dyDescent="0.25">
@@ -3559,9 +3458,8 @@
       <c r="C121" s="7">
         <v>500000</v>
       </c>
-      <c r="D121" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>32</v>
+      <c r="D121" s="4">
+        <v>26</v>
       </c>
     </row>
     <row r="122" spans="2:4" x14ac:dyDescent="0.25">
@@ -3569,11 +3467,10 @@
         <v>103</v>
       </c>
       <c r="C122" s="8">
-        <v>500000</v>
-      </c>
-      <c r="D122" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>29</v>
+        <v>351631</v>
+      </c>
+      <c r="D122" s="5">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>